<commit_message>
Xlsx template upload added
</commit_message>
<xml_diff>
--- a/public/Test Herbal Essences en-us.xlsx
+++ b/public/Test Herbal Essences en-us.xlsx
@@ -13,17 +13,17 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1644118163" val="1042" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1644118163" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1644118163" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1644118163"/>
+      <pm:revision xmlns:pm="smNativeData" day="1644772818" val="1042" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1644772818" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1644772818" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1644772818"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="203">
   <si>
     <t>Title</t>
   </si>
@@ -34,6 +34,9 @@
     <t>SKU</t>
   </si>
   <si>
+    <t>type</t>
+  </si>
+  <si>
     <t>mpId</t>
   </si>
   <si>
@@ -44,6 +47,9 @@
   </si>
   <si>
     <t>https://herbalessences.com/en-us/our-products/argan-oil/argan-oil-aloe-sulfate-hair-shampoo/</t>
+  </si>
+  <si>
+    <t>product</t>
   </si>
   <si>
     <t>Argan Oil &amp; Aloe Vera Sulfate-Free Conditioner</t>
@@ -650,7 +656,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -665,7 +671,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -680,23 +686,23 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="none" kern="1">
-            <pm:latin face="Calibri" sz="220" lang="default"/>
-            <pm:cs face="Basic Roman" sz="220" lang="default"/>
-            <pm:ea face="Basic Roman" sz="220" lang="default"/>
-          </pm:charSpec>
-        </ext>
-      </extLst>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="11"/>
-      <u val="single"/>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="none" kern="1">
+            <pm:latin face="Calibri" sz="220" lang="default"/>
+            <pm:cs face="Basic Roman" sz="220" lang="default"/>
+            <pm:ea face="Basic Roman" sz="220" lang="default"/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
+      <u val="single"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -713,7 +719,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -730,7 +736,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -747,7 +753,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -764,7 +770,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -781,7 +787,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -798,7 +804,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -815,7 +821,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -832,7 +838,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -849,7 +855,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -866,7 +872,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -883,7 +889,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -900,7 +906,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -917,7 +923,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -934,7 +940,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -951,7 +957,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -968,7 +974,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -985,7 +991,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1002,7 +1008,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1019,7 +1025,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1036,7 +1042,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1053,7 +1059,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1070,7 +1076,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1087,7 +1093,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1104,7 +1110,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1121,7 +1127,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1138,7 +1144,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1155,7 +1161,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1172,7 +1178,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1189,7 +1195,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1206,7 +1212,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1223,7 +1229,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1240,7 +1246,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1257,7 +1263,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1274,7 +1280,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1291,7 +1297,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1308,7 +1314,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1325,7 +1331,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1342,7 +1348,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1359,7 +1365,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1376,7 +1382,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1393,7 +1399,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1410,7 +1416,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1427,7 +1433,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1444,7 +1450,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1461,7 +1467,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1478,7 +1484,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1495,7 +1501,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1512,7 +1518,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1529,7 +1535,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1546,7 +1552,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1563,7 +1569,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1580,7 +1586,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1597,7 +1603,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1614,7 +1620,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1631,7 +1637,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1648,7 +1654,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1665,7 +1671,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1682,7 +1688,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1699,7 +1705,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1716,7 +1722,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1733,7 +1739,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1750,7 +1756,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1767,7 +1773,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1784,7 +1790,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1801,7 +1807,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1818,7 +1824,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1835,7 +1841,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1852,7 +1858,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1869,7 +1875,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1886,7 +1892,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1903,7 +1909,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1920,7 +1926,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1937,7 +1943,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1954,7 +1960,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1971,7 +1977,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1988,7 +1994,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2005,7 +2011,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2022,7 +2028,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2039,7 +2045,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2056,7 +2062,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2073,7 +2079,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2090,7 +2096,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2107,7 +2113,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2124,7 +2130,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2141,7 +2147,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2158,7 +2164,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2175,7 +2181,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2192,7 +2198,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2209,7 +2215,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2226,7 +2232,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2243,7 +2249,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2260,7 +2266,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2277,7 +2283,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2294,7 +2300,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2311,7 +2317,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2328,7 +2334,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2345,7 +2351,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1644118163" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1644772818" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -2379,7 +2385,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1644118163"/>
+          <pm:border xmlns:pm="smNativeData" id="1644772818"/>
         </ext>
       </extLst>
     </border>
@@ -2699,7 +2705,7 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1644118163" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1644772818" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
     </ext>
@@ -2966,10 +2972,10 @@
   <sheetPr>
     <outlinePr summaryRight="0" summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E99"/>
+  <dimension ref="A1:F99"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" view="normal" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="13" defaultColWidth="14.432432" defaultRowHeight="15.75" customHeight="1"/>
@@ -2978,7 +2984,7 @@
     <col min="2" max="2" width="118.567568" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2994,1476 +3000,1773 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="n">
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="n">
         <v>779532</v>
       </c>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="n">
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2" t="n">
         <v>779531</v>
       </c>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="D4" s="2" t="n">
+      <c r="D4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="2" t="n">
         <v>462741</v>
       </c>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="D5" s="2" t="n">
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="2" t="n">
         <v>462742</v>
       </c>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="D6" s="2" t="n">
+      <c r="D6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="2" t="n">
         <v>462732</v>
       </c>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="D7" s="2" t="n">
+      <c r="D7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="2" t="n">
         <v>462734</v>
       </c>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="D8" s="2" t="n">
+      <c r="D8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="2" t="n">
         <v>1032330</v>
       </c>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="D9" s="2" t="n">
+      <c r="D9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="2" t="n">
         <v>462738</v>
       </c>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="D10" s="2" t="n">
+      <c r="D10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="2" t="n">
         <v>462739</v>
       </c>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C11" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="D11" s="2" t="n">
+      <c r="D11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="2" t="n">
         <v>462740</v>
       </c>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="D12" s="2" t="n">
+      <c r="D12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="2" t="n">
         <v>462730</v>
       </c>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C13" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="D13" s="2" t="n">
+      <c r="D13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="2" t="n">
         <v>462743</v>
       </c>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C14" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="D14" s="2" t="n">
+      <c r="D14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="2" t="n">
         <v>462708</v>
       </c>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C15" s="2" t="n">
         <v>14</v>
       </c>
-      <c r="D15" s="2" t="n">
+      <c r="D15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="2" t="n">
         <v>794194</v>
       </c>
-      <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C16" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="D16" s="2" t="n">
+      <c r="D16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="2" t="n">
         <v>794188</v>
       </c>
-      <c r="E16" s="3"/>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C17" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="D17" s="2" t="n">
+      <c r="D17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="2" t="n">
         <v>776662</v>
       </c>
-      <c r="E17" s="3"/>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C18" s="2" t="n">
         <v>17</v>
       </c>
-      <c r="D18" s="2" t="n">
+      <c r="D18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="2" t="n">
         <v>794186</v>
       </c>
-      <c r="E18" s="3"/>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C19" s="2" t="n">
         <v>18</v>
       </c>
-      <c r="D19" s="2" t="n">
+      <c r="D19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="2" t="n">
         <v>865025</v>
       </c>
-      <c r="E19" s="3"/>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C20" s="2" t="n">
         <v>19</v>
       </c>
-      <c r="D20" s="2" t="n">
+      <c r="D20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="2" t="n">
         <v>389135</v>
       </c>
-      <c r="E20" s="3"/>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C21" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="D21" s="2" t="n">
+      <c r="D21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="2" t="n">
         <v>389123</v>
       </c>
-      <c r="E21" s="3"/>
-    </row>
-    <row r="22" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C22" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="D22" s="2" t="n">
+      <c r="D22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="2" t="n">
         <v>462744</v>
       </c>
-      <c r="E22" s="3"/>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C23" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="D23" s="2" t="n">
+      <c r="D23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="2" t="n">
         <v>462745</v>
       </c>
-      <c r="E23" s="3"/>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" spans="1:6" ht="15.75" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C24" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="D24" s="2" t="n">
+      <c r="D24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="2" t="n">
         <v>865017</v>
       </c>
-      <c r="E24" s="3"/>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B25" s="27" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C25" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="D25" s="2" t="n">
+      <c r="D25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="2" t="n">
         <v>776663</v>
       </c>
-      <c r="E25" s="3"/>
-    </row>
-    <row r="26" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B26" s="28" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C26" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="D26" s="2" t="n">
+      <c r="D26" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="2" t="n">
         <v>462729</v>
       </c>
-      <c r="E26" s="3"/>
-    </row>
-    <row r="27" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F26" s="3"/>
+    </row>
+    <row r="27" spans="1:6" ht="15.75" customHeight="1">
       <c r="A27" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B27" s="29" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C27" s="2" t="n">
         <v>26</v>
       </c>
-      <c r="D27" s="2" t="n">
+      <c r="D27" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="2" t="n">
         <v>462727</v>
       </c>
-      <c r="E27" s="3"/>
-    </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" spans="1:6" ht="15.75" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B28" s="30" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C28" s="2" t="n">
         <v>27</v>
       </c>
-      <c r="D28" s="2" t="n">
+      <c r="D28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="2" t="n">
         <v>389101</v>
       </c>
-      <c r="E28" s="3"/>
-    </row>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F28" s="3"/>
+    </row>
+    <row r="29" spans="1:6" ht="15.75" customHeight="1">
       <c r="A29" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B29" s="31" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C29" s="2" t="n">
         <v>28</v>
       </c>
-      <c r="D29" s="2" t="n">
+      <c r="D29" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="2" t="n">
         <v>389092</v>
       </c>
-      <c r="E29" s="3"/>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F29" s="3"/>
+    </row>
+    <row r="30" spans="1:6" ht="15.75" customHeight="1">
       <c r="A30" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B30" s="32" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C30" s="2" t="n">
         <v>29</v>
       </c>
-      <c r="D30" s="2" t="n">
+      <c r="D30" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="2" t="n">
         <v>462724</v>
       </c>
-      <c r="E30" s="3"/>
-    </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F30" s="3"/>
+    </row>
+    <row r="31" spans="1:6" ht="15.75" customHeight="1">
       <c r="A31" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B31" s="33" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C31" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="D31" s="2" t="n">
+      <c r="D31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="2" t="n">
         <v>462719</v>
       </c>
-      <c r="E31" s="3"/>
-    </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F31" s="3"/>
+    </row>
+    <row r="32" spans="1:6" ht="15.75" customHeight="1">
       <c r="A32" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B32" s="34" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C32" s="2" t="n">
         <v>31</v>
       </c>
-      <c r="D32" s="2" t="n">
+      <c r="D32" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="2" t="n">
         <v>434024</v>
       </c>
-      <c r="E32" s="3"/>
-    </row>
-    <row r="33" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F32" s="3"/>
+    </row>
+    <row r="33" spans="1:6" ht="15.75" customHeight="1">
       <c r="A33" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B33" s="35" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C33" s="2" t="n">
         <v>32</v>
       </c>
-      <c r="D33" s="2" t="n">
+      <c r="D33" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" s="2" t="n">
         <v>776664</v>
       </c>
-      <c r="E33" s="3"/>
-    </row>
-    <row r="34" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F33" s="3"/>
+    </row>
+    <row r="34" spans="1:6" ht="15.75" customHeight="1">
       <c r="A34" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B34" s="36" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C34" s="2" t="n">
         <v>33</v>
       </c>
-      <c r="D34" s="2" t="n">
+      <c r="D34" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="2" t="n">
         <v>462728</v>
       </c>
-      <c r="E34" s="3"/>
-    </row>
-    <row r="35" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F34" s="3"/>
+    </row>
+    <row r="35" spans="1:6" ht="15.75" customHeight="1">
       <c r="A35" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B35" s="37" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C35" s="2" t="n">
         <v>34</v>
       </c>
-      <c r="D35" s="2" t="n">
+      <c r="D35" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" s="2" t="n">
         <v>389073</v>
       </c>
-      <c r="E35" s="3"/>
-    </row>
-    <row r="36" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F35" s="3"/>
+    </row>
+    <row r="36" spans="1:6" ht="15.75" customHeight="1">
       <c r="A36" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B36" s="38" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C36" s="2" t="n">
         <v>35</v>
       </c>
-      <c r="D36" s="2" t="n">
+      <c r="D36" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" s="2" t="n">
         <v>389065</v>
       </c>
-      <c r="E36" s="3"/>
-    </row>
-    <row r="37" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F36" s="3"/>
+    </row>
+    <row r="37" spans="1:6" ht="15.75" customHeight="1">
       <c r="A37" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B37" s="39" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C37" s="2" t="n">
         <v>36</v>
       </c>
-      <c r="D37" s="2" t="n">
+      <c r="D37" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="2" t="n">
         <v>1023721</v>
       </c>
-      <c r="E37" s="3"/>
-    </row>
-    <row r="38" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F37" s="3"/>
+    </row>
+    <row r="38" spans="1:6" ht="15.75" customHeight="1">
       <c r="A38" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B38" s="40" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C38" s="2" t="n">
         <v>37</v>
       </c>
-      <c r="D38" s="2" t="n">
+      <c r="D38" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" s="2" t="n">
         <v>776643</v>
       </c>
-      <c r="E38" s="3"/>
-    </row>
-    <row r="39" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F38" s="3"/>
+    </row>
+    <row r="39" spans="1:6" ht="15.75" customHeight="1">
       <c r="A39" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B39" s="41" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C39" s="2" t="n">
         <v>38</v>
       </c>
-      <c r="D39" s="2" t="n">
+      <c r="D39" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" s="2" t="n">
         <v>395908</v>
       </c>
-      <c r="E39" s="3"/>
-    </row>
-    <row r="40" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F39" s="3"/>
+    </row>
+    <row r="40" spans="1:6" ht="15.75" customHeight="1">
       <c r="A40" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B40" s="42" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C40" s="2" t="n">
         <v>39</v>
       </c>
-      <c r="D40" s="2" t="n">
+      <c r="D40" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" s="2" t="n">
         <v>389038</v>
       </c>
-      <c r="E40" s="3"/>
-    </row>
-    <row r="41" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F40" s="3"/>
+    </row>
+    <row r="41" spans="1:6" ht="15.75" customHeight="1">
       <c r="A41" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B41" s="43" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C41" s="2" t="n">
         <v>40</v>
       </c>
-      <c r="D41" s="2" t="n">
+      <c r="D41" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" s="2" t="n">
         <v>389086</v>
       </c>
-      <c r="E41" s="3"/>
-    </row>
-    <row r="42" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F41" s="3"/>
+    </row>
+    <row r="42" spans="1:6" ht="15.75" customHeight="1">
       <c r="A42" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B42" s="44" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C42" s="2" t="n">
         <v>41</v>
       </c>
-      <c r="D42" s="2" t="n">
+      <c r="D42" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" s="2" t="n">
         <v>389081</v>
       </c>
-      <c r="E42" s="3"/>
-    </row>
-    <row r="43" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F42" s="3"/>
+    </row>
+    <row r="43" spans="1:6" ht="15.75" customHeight="1">
       <c r="A43" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B43" s="45" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C43" s="2" t="n">
         <v>42</v>
       </c>
-      <c r="D43" s="2" t="n">
+      <c r="D43" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43" s="2" t="n">
         <v>462715</v>
       </c>
-      <c r="E43" s="3"/>
-    </row>
-    <row r="44" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F43" s="3"/>
+    </row>
+    <row r="44" spans="1:6" ht="15.75" customHeight="1">
       <c r="A44" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B44" s="46" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C44" s="2" t="n">
         <v>43</v>
       </c>
-      <c r="D44" s="2" t="n">
+      <c r="D44" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" s="2" t="n">
         <v>462691</v>
       </c>
-      <c r="E44" s="3"/>
-    </row>
-    <row r="45" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F44" s="3"/>
+    </row>
+    <row r="45" spans="1:6" ht="15.75" customHeight="1">
       <c r="A45" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B45" s="47" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C45" s="2" t="n">
         <v>44</v>
       </c>
-      <c r="D45" s="2" t="n">
+      <c r="D45" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E45" s="2" t="n">
         <v>462671</v>
       </c>
-      <c r="E45" s="3"/>
-    </row>
-    <row r="46" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F45" s="3"/>
+    </row>
+    <row r="46" spans="1:6" ht="15.75" customHeight="1">
       <c r="A46" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B46" s="48" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C46" s="2" t="n">
         <v>45</v>
       </c>
-      <c r="D46" s="2" t="n">
+      <c r="D46" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46" s="2" t="n">
         <v>389119</v>
       </c>
-      <c r="E46" s="3"/>
-    </row>
-    <row r="47" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F46" s="3"/>
+    </row>
+    <row r="47" spans="1:6" ht="15.75" customHeight="1">
       <c r="A47" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B47" s="49" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C47" s="2" t="n">
         <v>46</v>
       </c>
-      <c r="D47" s="2" t="n">
+      <c r="D47" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E47" s="2" t="n">
         <v>389108</v>
       </c>
-      <c r="E47" s="3"/>
-    </row>
-    <row r="48" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F47" s="3"/>
+    </row>
+    <row r="48" spans="1:6" ht="15.75" customHeight="1">
       <c r="A48" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B48" s="50" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C48" s="2" t="n">
         <v>47</v>
       </c>
-      <c r="D48" s="2" t="n">
+      <c r="D48" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" s="2" t="n">
         <v>776650</v>
       </c>
-      <c r="E48" s="3"/>
-    </row>
-    <row r="49" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F48" s="3"/>
+    </row>
+    <row r="49" spans="1:6" ht="15.75" customHeight="1">
       <c r="A49" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B49" s="51" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C49" s="2" t="n">
         <v>48</v>
       </c>
-      <c r="D49" s="2" t="n">
+      <c r="D49" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E49" s="2" t="n">
         <v>389030</v>
       </c>
-      <c r="E49" s="3"/>
-    </row>
-    <row r="50" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F49" s="3"/>
+    </row>
+    <row r="50" spans="1:6" ht="15.75" customHeight="1">
       <c r="A50" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B50" s="52" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C50" s="2" t="n">
         <v>49</v>
       </c>
-      <c r="D50" s="2" t="n">
+      <c r="D50" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E50" s="2" t="n">
         <v>389023</v>
       </c>
-      <c r="E50" s="3"/>
-    </row>
-    <row r="51" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F50" s="3"/>
+    </row>
+    <row r="51" spans="1:6" ht="15.75" customHeight="1">
       <c r="A51" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B51" s="53" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C51" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="D51" s="2" t="n">
+      <c r="D51" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E51" s="2" t="n">
         <v>389048</v>
       </c>
-      <c r="E51" s="3"/>
-    </row>
-    <row r="52" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F51" s="3"/>
+    </row>
+    <row r="52" spans="1:6" ht="15.75" customHeight="1">
       <c r="A52" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B52" s="54" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C52" s="2" t="n">
         <v>51</v>
       </c>
-      <c r="D52" s="2" t="n">
+      <c r="D52" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E52" s="2" t="n">
         <v>389062</v>
       </c>
-      <c r="E52" s="3"/>
-    </row>
-    <row r="53" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F52" s="3"/>
+    </row>
+    <row r="53" spans="1:6" ht="15.75" customHeight="1">
       <c r="A53" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B53" s="55" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C53" s="2" t="n">
         <v>52</v>
       </c>
-      <c r="D53" s="2" t="n">
+      <c r="D53" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E53" s="2" t="n">
         <v>389059</v>
       </c>
-      <c r="E53" s="3"/>
-    </row>
-    <row r="54" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F53" s="3"/>
+    </row>
+    <row r="54" spans="1:6" ht="15.75" customHeight="1">
       <c r="A54" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B54" s="56" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C54" s="2" t="n">
         <v>53</v>
       </c>
-      <c r="D54" s="2" t="n">
+      <c r="D54" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E54" s="2" t="n">
         <v>462704</v>
       </c>
-      <c r="E54" s="3"/>
-    </row>
-    <row r="55" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F54" s="3"/>
+    </row>
+    <row r="55" spans="1:6" ht="15.75" customHeight="1">
       <c r="A55" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B55" s="57" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C55" s="2" t="n">
         <v>54</v>
       </c>
-      <c r="D55" s="2" t="n">
+      <c r="D55" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E55" s="2" t="n">
         <v>462677</v>
       </c>
-      <c r="E55" s="3"/>
-    </row>
-    <row r="56" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F55" s="3"/>
+    </row>
+    <row r="56" spans="1:6" ht="15.75" customHeight="1">
       <c r="A56" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B56" s="58" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C56" s="2" t="n">
         <v>55</v>
       </c>
-      <c r="D56" s="2" t="n">
+      <c r="D56" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E56" s="2" t="n">
         <v>462721</v>
       </c>
-      <c r="E56" s="3"/>
-    </row>
-    <row r="57" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F56" s="3"/>
+    </row>
+    <row r="57" spans="1:6" ht="15.75" customHeight="1">
       <c r="A57" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B57" s="59" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C57" s="2" t="n">
         <v>56</v>
       </c>
-      <c r="D57" s="2" t="n">
+      <c r="D57" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E57" s="2" t="n">
         <v>462720</v>
       </c>
-      <c r="E57" s="3"/>
-    </row>
-    <row r="58" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F57" s="3"/>
+    </row>
+    <row r="58" spans="1:6" ht="15.75" customHeight="1">
       <c r="A58" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B58" s="60" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C58" s="2" t="n">
         <v>57</v>
       </c>
-      <c r="D58" s="2" t="n">
+      <c r="D58" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E58" s="2" t="n">
         <v>462711</v>
       </c>
-      <c r="E58" s="3"/>
-    </row>
-    <row r="59" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F58" s="3"/>
+    </row>
+    <row r="59" spans="1:6" ht="15.75" customHeight="1">
       <c r="A59" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B59" s="61" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C59" s="2" t="n">
         <v>58</v>
       </c>
-      <c r="D59" s="2" t="n">
+      <c r="D59" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E59" s="2" t="n">
         <v>462696</v>
       </c>
-      <c r="E59" s="3"/>
-    </row>
-    <row r="60" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F59" s="3"/>
+    </row>
+    <row r="60" spans="1:6" ht="15.75" customHeight="1">
       <c r="A60" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B60" s="62" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C60" s="2" t="n">
         <v>59</v>
       </c>
-      <c r="D60" s="2" t="n">
+      <c r="D60" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E60" s="2" t="n">
         <v>462700</v>
       </c>
-      <c r="E60" s="3"/>
-    </row>
-    <row r="61" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F60" s="3"/>
+    </row>
+    <row r="61" spans="1:6" ht="15.75" customHeight="1">
       <c r="A61" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B61" s="63" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C61" s="2" t="n">
         <v>60</v>
       </c>
-      <c r="D61" s="2" t="n">
+      <c r="D61" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E61" s="2" t="n">
         <v>389012</v>
       </c>
-      <c r="E61" s="3"/>
-    </row>
-    <row r="62" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F61" s="3"/>
+    </row>
+    <row r="62" spans="1:6" ht="15.75" customHeight="1">
       <c r="A62" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B62" s="64" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C62" s="2" t="n">
         <v>61</v>
       </c>
-      <c r="D62" s="2" t="n">
+      <c r="D62" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E62" s="2" t="n">
         <v>389051</v>
       </c>
-      <c r="E62" s="3"/>
-    </row>
-    <row r="63" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F62" s="3"/>
+    </row>
+    <row r="63" spans="1:6" ht="15.75" customHeight="1">
       <c r="A63" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B63" s="65" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C63" s="2" t="n">
         <v>62</v>
       </c>
-      <c r="D63" s="2" t="n">
+      <c r="D63" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E63" s="2" t="n">
         <v>1023722</v>
       </c>
-      <c r="E63" s="3"/>
-    </row>
-    <row r="64" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F63" s="3"/>
+    </row>
+    <row r="64" spans="1:6" ht="15.75" customHeight="1">
       <c r="A64" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B64" s="66" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C64" s="2" t="n">
         <v>63</v>
       </c>
-      <c r="D64" s="2" t="n">
+      <c r="D64" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E64" s="2" t="n">
         <v>794169</v>
       </c>
-      <c r="E64" s="3"/>
-    </row>
-    <row r="65" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F64" s="3"/>
+    </row>
+    <row r="65" spans="1:6" ht="15.75" customHeight="1">
       <c r="A65" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B65" s="67" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C65" s="2" t="n">
         <v>64</v>
       </c>
-      <c r="D65" s="2" t="n">
+      <c r="D65" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E65" s="2" t="n">
         <v>462736</v>
       </c>
-      <c r="E65" s="3"/>
-    </row>
-    <row r="66" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F65" s="3"/>
+    </row>
+    <row r="66" spans="1:6" ht="15.75" customHeight="1">
       <c r="A66" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B66" s="68" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C66" s="2" t="n">
         <v>65</v>
       </c>
-      <c r="D66" s="2" t="n">
+      <c r="D66" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E66" s="2" t="n">
         <v>794198</v>
       </c>
-      <c r="E66" s="3"/>
-    </row>
-    <row r="67" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F66" s="3"/>
+    </row>
+    <row r="67" spans="1:6" ht="15.75" customHeight="1">
       <c r="A67" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B67" s="69" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C67" s="2" t="n">
         <v>66</v>
       </c>
-      <c r="D67" s="2" t="n">
+      <c r="D67" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E67" s="2" t="n">
         <v>794190</v>
       </c>
-      <c r="E67" s="3"/>
-    </row>
-    <row r="68" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F67" s="3"/>
+    </row>
+    <row r="68" spans="1:6" ht="15.75" customHeight="1">
       <c r="A68" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B68" s="70" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C68" s="2" t="n">
         <v>67</v>
       </c>
-      <c r="D68" s="2" t="n">
+      <c r="D68" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E68" s="2" t="n">
         <v>865027</v>
       </c>
-      <c r="E68" s="3"/>
-    </row>
-    <row r="69" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F68" s="3"/>
+    </row>
+    <row r="69" spans="1:6" ht="15.75" customHeight="1">
       <c r="A69" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B69" s="71" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C69" s="2" t="n">
         <v>68</v>
       </c>
-      <c r="D69" s="2" t="n">
+      <c r="D69" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E69" s="2" t="n">
         <v>865028</v>
       </c>
-      <c r="E69" s="3"/>
-    </row>
-    <row r="70" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F69" s="3"/>
+    </row>
+    <row r="70" spans="1:6" ht="15.75" customHeight="1">
       <c r="A70" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B70" s="72" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C70" s="2" t="n">
         <v>69</v>
       </c>
-      <c r="D70" s="2" t="n">
+      <c r="D70" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E70" s="2" t="n">
         <v>462757</v>
       </c>
-      <c r="E70" s="3"/>
-    </row>
-    <row r="71" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F70" s="3"/>
+    </row>
+    <row r="71" spans="1:6" ht="15.75" customHeight="1">
       <c r="A71" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B71" s="73" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C71" s="2" t="n">
         <v>70</v>
       </c>
-      <c r="D71" s="2" t="n">
+      <c r="D71" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E71" s="2" t="n">
         <v>467893</v>
       </c>
-      <c r="E71" s="3"/>
-    </row>
-    <row r="72" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F71" s="3"/>
+    </row>
+    <row r="72" spans="1:6" ht="15.75" customHeight="1">
       <c r="A72" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B72" s="74" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C72" s="2" t="n">
         <v>71</v>
       </c>
-      <c r="D72" s="2" t="n">
+      <c r="D72" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E72" s="2" t="n">
         <v>462803</v>
       </c>
-      <c r="E72" s="3"/>
-    </row>
-    <row r="73" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F72" s="3"/>
+    </row>
+    <row r="73" spans="1:6" ht="15.75" customHeight="1">
       <c r="A73" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B73" s="75" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C73" s="2" t="n">
         <v>72</v>
       </c>
-      <c r="D73" s="2" t="n">
+      <c r="D73" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E73" s="2" t="n">
         <v>462758</v>
       </c>
-      <c r="E73" s="3"/>
-    </row>
-    <row r="74" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F73" s="3"/>
+    </row>
+    <row r="74" spans="1:6" ht="15.75" customHeight="1">
       <c r="A74" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B74" s="76" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C74" s="2" t="n">
         <v>73</v>
       </c>
-      <c r="D74" s="2" t="n">
+      <c r="D74" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E74" s="2" t="n">
         <v>462810</v>
       </c>
-      <c r="E74" s="3"/>
-    </row>
-    <row r="75" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F74" s="3"/>
+    </row>
+    <row r="75" spans="1:6" ht="15.75" customHeight="1">
       <c r="A75" s="1" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B75" s="77" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C75" s="2" t="n">
         <v>74</v>
       </c>
-      <c r="D75" s="2" t="n">
+      <c r="D75" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E75" s="2" t="n">
         <v>462819</v>
       </c>
-      <c r="E75" s="3"/>
-    </row>
-    <row r="76" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F75" s="3"/>
+    </row>
+    <row r="76" spans="1:6" ht="15.75" customHeight="1">
       <c r="A76" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B76" s="78" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C76" s="2" t="n">
         <v>75</v>
       </c>
-      <c r="D76" s="2" t="n">
+      <c r="D76" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E76" s="2" t="n">
         <v>462833</v>
       </c>
-      <c r="E76" s="3"/>
-    </row>
-    <row r="77" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F76" s="3"/>
+    </row>
+    <row r="77" spans="1:6" ht="15.75" customHeight="1">
       <c r="A77" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B77" s="79" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C77" s="2" t="n">
         <v>76</v>
       </c>
-      <c r="D77" s="2" t="n">
+      <c r="D77" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E77" s="2" t="n">
         <v>462685</v>
       </c>
-      <c r="E77" s="3"/>
-    </row>
-    <row r="78" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F77" s="3"/>
+    </row>
+    <row r="78" spans="1:6" ht="15.75" customHeight="1">
       <c r="A78" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B78" s="80" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C78" s="2" t="n">
         <v>77</v>
       </c>
-      <c r="D78" s="2" t="n">
+      <c r="D78" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E78" s="2" t="n">
         <v>776608</v>
       </c>
-      <c r="E78" s="3"/>
-    </row>
-    <row r="79" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F78" s="3"/>
+    </row>
+    <row r="79" spans="1:6" ht="15.75" customHeight="1">
       <c r="A79" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B79" s="81" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C79" s="2" t="n">
         <v>78</v>
       </c>
-      <c r="D79" s="2" t="n">
+      <c r="D79" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E79" s="2" t="n">
         <v>776618</v>
       </c>
-      <c r="E79" s="3"/>
-    </row>
-    <row r="80" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F79" s="3"/>
+    </row>
+    <row r="80" spans="1:6" ht="15.75" customHeight="1">
       <c r="A80" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B80" s="82" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C80" s="2" t="n">
         <v>79</v>
       </c>
-      <c r="D80" s="2" t="n">
+      <c r="D80" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E80" s="2" t="n">
         <v>776633</v>
       </c>
-      <c r="E80" s="3"/>
-    </row>
-    <row r="81" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F80" s="3"/>
+    </row>
+    <row r="81" spans="1:6" ht="15.75" customHeight="1">
       <c r="A81" s="1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B81" s="83" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C81" s="2" t="n">
         <v>80</v>
       </c>
-      <c r="D81" s="2" t="n">
+      <c r="D81" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E81" s="2" t="n">
         <v>794183</v>
       </c>
-      <c r="E81" s="3"/>
-    </row>
-    <row r="82" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F81" s="3"/>
+    </row>
+    <row r="82" spans="1:6" ht="15.75" customHeight="1">
       <c r="A82" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B82" s="84" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C82" s="2" t="n">
         <v>81</v>
       </c>
-      <c r="D82" s="2" t="n">
+      <c r="D82" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E82" s="2" t="n">
         <v>794182</v>
       </c>
-      <c r="E82" s="3"/>
-    </row>
-    <row r="83" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F82" s="3"/>
+    </row>
+    <row r="83" spans="1:6" ht="15.75" customHeight="1">
       <c r="A83" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B83" s="85" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C83" s="2" t="n">
         <v>82</v>
       </c>
-      <c r="D83" s="2" t="n">
+      <c r="D83" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E83" s="2" t="n">
         <v>776626</v>
       </c>
-      <c r="E83" s="3"/>
-    </row>
-    <row r="84" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F83" s="3"/>
+    </row>
+    <row r="84" spans="1:6" ht="15.75" customHeight="1">
       <c r="A84" s="1" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B84" s="86" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C84" s="2" t="n">
         <v>83</v>
       </c>
-      <c r="D84" s="2" t="n">
+      <c r="D84" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E84" s="2" t="n">
         <v>776665</v>
       </c>
-      <c r="E84" s="3"/>
-    </row>
-    <row r="85" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F84" s="3"/>
+    </row>
+    <row r="85" spans="1:6" ht="15.75" customHeight="1">
       <c r="A85" s="1" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B85" s="87" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C85" s="2" t="n">
         <v>84</v>
       </c>
-      <c r="D85" s="2" t="n">
+      <c r="D85" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E85" s="2" t="n">
         <v>389431</v>
       </c>
-      <c r="E85" s="3"/>
-    </row>
-    <row r="86" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F85" s="3"/>
+    </row>
+    <row r="86" spans="1:6" ht="15.75" customHeight="1">
       <c r="A86" s="1" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B86" s="88" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C86" s="2" t="n">
         <v>85</v>
       </c>
-      <c r="D86" s="2" t="n">
+      <c r="D86" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E86" s="2" t="n">
         <v>776606</v>
       </c>
-      <c r="E86" s="3"/>
-    </row>
-    <row r="87" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F86" s="3"/>
+    </row>
+    <row r="87" spans="1:6" ht="15.75" customHeight="1">
       <c r="A87" s="1" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B87" s="89" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C87" s="2" t="n">
         <v>86</v>
       </c>
-      <c r="D87" s="2" t="n">
+      <c r="D87" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E87" s="2" t="n">
         <v>776590</v>
       </c>
-      <c r="E87" s="3"/>
-    </row>
-    <row r="88" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F87" s="3"/>
+    </row>
+    <row r="88" spans="1:6" ht="15.75" customHeight="1">
       <c r="A88" s="1" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B88" s="90" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C88" s="2" t="n">
         <v>87</v>
       </c>
-      <c r="D88" s="2" t="n">
+      <c r="D88" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E88" s="2" t="n">
         <v>776669</v>
       </c>
-      <c r="E88" s="3"/>
-    </row>
-    <row r="89" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F88" s="3"/>
+    </row>
+    <row r="89" spans="1:6" ht="15.75" customHeight="1">
       <c r="A89" s="1" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B89" s="91" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C89" s="2" t="n">
         <v>88</v>
       </c>
-      <c r="D89" s="2" t="n">
+      <c r="D89" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E89" s="2" t="n">
         <v>776644</v>
       </c>
-      <c r="E89" s="3"/>
-    </row>
-    <row r="90" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F89" s="3"/>
+    </row>
+    <row r="90" spans="1:6" ht="15.75" customHeight="1">
       <c r="A90" s="1" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B90" s="92" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C90" s="2" t="n">
         <v>89</v>
       </c>
-      <c r="D90" s="2" t="n">
+      <c r="D90" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E90" s="2" t="n">
         <v>389423</v>
       </c>
-      <c r="E90" s="3"/>
-    </row>
-    <row r="91" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F90" s="3"/>
+    </row>
+    <row r="91" spans="1:6" ht="15.75" customHeight="1">
       <c r="A91" s="1" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B91" s="93" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C91" s="2" t="n">
         <v>90</v>
       </c>
-      <c r="D91" s="2" t="n">
+      <c r="D91" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E91" s="2" t="n">
         <v>776592</v>
       </c>
-      <c r="E91" s="3"/>
-    </row>
-    <row r="92" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F91" s="3"/>
+    </row>
+    <row r="92" spans="1:6" ht="15.75" customHeight="1">
       <c r="A92" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B92" s="94" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C92" s="2" t="n">
         <v>91</v>
       </c>
-      <c r="D92" s="2" t="n">
+      <c r="D92" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E92" s="2" t="n">
         <v>776671</v>
       </c>
-      <c r="E92" s="3"/>
-    </row>
-    <row r="93" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F92" s="3"/>
+    </row>
+    <row r="93" spans="1:6" ht="15.75" customHeight="1">
       <c r="A93" s="1" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B93" s="95" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C93" s="2" t="n">
         <v>92</v>
       </c>
-      <c r="D93" s="2" t="n">
+      <c r="D93" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E93" s="2" t="n">
         <v>776670</v>
       </c>
-      <c r="E93" s="3"/>
-    </row>
-    <row r="94" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F93" s="3"/>
+    </row>
+    <row r="94" spans="1:6" ht="15.75" customHeight="1">
       <c r="A94" s="1" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B94" s="96" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C94" s="2" t="n">
         <v>93</v>
       </c>
-      <c r="D94" s="2" t="n">
+      <c r="D94" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E94" s="2" t="n">
         <v>794202</v>
       </c>
-      <c r="E94" s="3"/>
-    </row>
-    <row r="95" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F94" s="3"/>
+    </row>
+    <row r="95" spans="1:6" ht="15.75" customHeight="1">
       <c r="A95" s="1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B95" s="97" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C95" s="2" t="n">
         <v>94</v>
       </c>
-      <c r="D95" s="2" t="n">
+      <c r="D95" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E95" s="2" t="n">
         <v>794201</v>
       </c>
-      <c r="E95" s="3"/>
-    </row>
-    <row r="96" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F95" s="3"/>
+    </row>
+    <row r="96" spans="1:6" ht="15.75" customHeight="1">
       <c r="A96" s="1" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B96" s="98" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C96" s="2" t="n">
         <v>95</v>
       </c>
-      <c r="D96" s="2" t="n">
+      <c r="D96" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E96" s="2" t="n">
         <v>1023727</v>
       </c>
-      <c r="E96" s="3"/>
-    </row>
-    <row r="97" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F96" s="3"/>
+    </row>
+    <row r="97" spans="1:6" ht="15.75" customHeight="1">
       <c r="A97" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B97" s="99" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C97" s="2" t="n">
         <v>96</v>
       </c>
-      <c r="D97" s="2" t="n">
+      <c r="D97" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E97" s="2" t="n">
         <v>794181</v>
       </c>
-      <c r="E97" s="3"/>
-    </row>
-    <row r="98" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F97" s="3"/>
+    </row>
+    <row r="98" spans="1:6" ht="15.75" customHeight="1">
       <c r="A98" s="1" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B98" s="100" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C98" s="2" t="n">
         <v>97</v>
       </c>
-      <c r="D98" s="2" t="n">
+      <c r="D98" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E98" s="2" t="n">
         <v>794200</v>
       </c>
-      <c r="E98" s="3"/>
-    </row>
-    <row r="99" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F98" s="3"/>
+    </row>
+    <row r="99" spans="1:6" ht="15.75" customHeight="1">
       <c r="A99" s="1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B99" s="101" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C99" s="2" t="n">
         <v>98</v>
       </c>
-      <c r="D99" s="2" t="n">
+      <c r="D99" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E99" s="2" t="n">
         <v>794177</v>
       </c>
-      <c r="E99" s="3"/>
+      <c r="F99" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4569,7 +4872,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1644118163" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1644772818" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -4578,14 +4881,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1644118163" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1644118163" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1644772818" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1644772818" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1644118163" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1644772818" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>